<commit_message>
Updated Docs for Presentation
</commit_message>
<xml_diff>
--- a/proj_asic/docs/budget.xlsx
+++ b/proj_asic/docs/budget.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Item</t>
   </si>
@@ -41,9 +41,6 @@
     <t>CORE 9 University</t>
   </si>
   <si>
-    <t>Mounting Hardware</t>
-  </si>
-  <si>
     <t>CY8CKIT-050 PSoC 5LP Development Kit</t>
   </si>
   <si>
@@ -53,10 +50,10 @@
     <t>Electronic Design Automation Tools</t>
   </si>
   <si>
-    <t>??</t>
-  </si>
-  <si>
     <t>Field Programmable Gate Array (FPGA)</t>
+  </si>
+  <si>
+    <t>Crystal Oscillators</t>
   </si>
 </sst>
 </file>
@@ -583,7 +580,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,10 +599,10 @@
     </row>
     <row r="2" spans="1:3" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -634,23 +631,23 @@
     </row>
     <row r="6" spans="1:3" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B6" s="4">
-        <v>100</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" s="12">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="14">
         <v>0</v>
@@ -658,11 +655,11 @@
     </row>
     <row r="9" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="16">
         <f>SUM(B3:B8)</f>
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="C9" s="2"/>
     </row>

</xml_diff>

<commit_message>
Updated Schedule and Budget
</commit_message>
<xml_diff>
--- a/proj_asic/docs/budget.xlsx
+++ b/proj_asic/docs/budget.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Item</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>Crystal Oscillators</t>
+  </si>
+  <si>
+    <t>UDA 1380 Board</t>
   </si>
 </sst>
 </file>
@@ -249,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -285,16 +288,22 @@
     <xf numFmtId="8" fontId="1" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="1" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="1" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="1" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="1" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="1" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -577,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,23 +654,31 @@
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B9" s="16">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="15" t="s">
+    <row r="10" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="16">
-        <f>SUM(B3:B8)</f>
-        <v>200</v>
-      </c>
-      <c r="C9" s="2"/>
+      <c r="B10" s="17">
+        <f>SUM(B3:B9)</f>
+        <v>220</v>
+      </c>
+      <c r="C10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>